<commit_message>
allora website automation setup
</commit_message>
<xml_diff>
--- a/Bonmillette_hybrid_framework_automation/excel_data/project_documents.xlsx
+++ b/Bonmillette_hybrid_framework_automation/excel_data/project_documents.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34E5F12-BFCD-49CE-8B6D-CFA37EB056E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8D045B-57D6-451D-B146-66C2B2A9BDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
     <t>http://localhost:5173/about-us</t>
   </si>
   <si>
-    <t>Homepage - Bonmillettes</t>
+    <t>Homepage - Bonmillette</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>